<commit_message>
1.5 peptoid screen + thickness photos
</commit_message>
<xml_diff>
--- a/r-code/18.3 software-dictionary.xlsx
+++ b/r-code/18.3 software-dictionary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64204\Desktop\master\r-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE3532A-B195-4980-A89D-F8BDAD583F25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAFB86D-2617-4FBC-9B6D-9A04E2846ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Type</t>
   </si>
@@ -115,6 +115,18 @@
   </si>
   <si>
     <t>Plot facetting</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>imageJ</t>
+  </si>
+  <si>
+    <t>1.54p</t>
+  </si>
+  <si>
+    <t>Fluorescence overlay</t>
   </si>
 </sst>
 </file>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,6 +578,20 @@
         <v>29</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
previous week upload images
</commit_message>
<xml_diff>
--- a/r-code/18.3 software-dictionary.xlsx
+++ b/r-code/18.3 software-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64204\Desktop\master\r-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAFB86D-2617-4FBC-9B6D-9A04E2846ED4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497DE1CE-4A92-485B-A937-D0F6F86099A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>Type</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>Fluorescence overlay</t>
+  </si>
+  <si>
+    <t>clusterProfiler</t>
+  </si>
+  <si>
+    <t>4.10.0</t>
+  </si>
+  <si>
+    <t>Genetic annotation</t>
+  </si>
+  <si>
+    <t>SnapGene</t>
+  </si>
+  <si>
+    <t>8.0.3</t>
+  </si>
+  <si>
+    <t>Plasmid map viewing and annotation (free version)</t>
   </si>
 </sst>
 </file>
@@ -444,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,6 +610,34 @@
         <v>33</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
images from prelim 1.
</commit_message>
<xml_diff>
--- a/r-code/18.3 software-dictionary.xlsx
+++ b/r-code/18.3 software-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\64204\Desktop\master\r-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497DE1CE-4A92-485B-A937-D0F6F86099A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{899929BB-4E28-40D8-90D7-67CAB31DB786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>Type</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Plasmid map viewing and annotation (free version)</t>
+  </si>
+  <si>
+    <t>colabfold</t>
+  </si>
+  <si>
+    <t>Notebook</t>
+  </si>
+  <si>
+    <t>1.5.5</t>
+  </si>
+  <si>
+    <t>GUI to alphafold</t>
   </si>
 </sst>
 </file>
@@ -462,7 +474,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
@@ -638,6 +650,20 @@
         <v>39</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>